<commit_message>
Checked LLM corrections and added notes
</commit_message>
<xml_diff>
--- a/data/llm_correction_check/llm_correction_checked.xlsx
+++ b/data/llm_correction_check/llm_correction_checked.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Dokumente\GitHub Desktop\nonsig-master-thesis\data\llm_correction_check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{636CDB6C-E091-43A1-BF97-052A20586D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE67F0D-F2D9-44C8-9FD0-17196BF59F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11235" yWindow="6165" windowWidth="21600" windowHeight="11295" xr2:uid="{2E904296-79A5-4A5C-B72F-CFC29AE77F1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2E904296-79A5-4A5C-B72F-CFC29AE77F1A}"/>
   </bookViews>
   <sheets>
-    <sheet name="llm_correction_unchecked" sheetId="1" r:id="rId1"/>
+    <sheet name="llm_correction_checked" sheetId="1" r:id="rId1"/>
+    <sheet name="codebook" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="242">
   <si>
     <t>statement</t>
   </si>
@@ -629,6 +643,127 @@
   </si>
   <si>
     <t>As expected on the basis of previous studies, t tests showed that there were no significant differences between groups on tests of either verbal, t(50) = 0.93, p = .36, or visual, t(50) = 1.00, p = .32, recognition memory of the film (Table S1 in the Supplemental Material)-this is consistent with the possibility that intrusivememory frequency (diary/IPT intrusion score) was influenced while leaving recognition memory (for facts and scenes in the trauma film) intact.</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>correction_correct</t>
+  </si>
+  <si>
+    <t>Originally extracted statement (from training data)</t>
+  </si>
+  <si>
+    <t>Corrected version of the sentence from the LLM</t>
+  </si>
+  <si>
+    <t>Human label whether the statement is correct:
+0 = Statement is correct and implies no absence of an effect
+1 = Statement is incorrect and implies the absence of an effect</t>
+  </si>
+  <si>
+    <t>Human label whether the LLM's correction is actually correct:
+0 = Statement is correct and implies no absence of an effect
+1 = Statement is incorrect and implies the absence of an effect</t>
+  </si>
+  <si>
+    <t>corrected_correct</t>
+  </si>
+  <si>
+    <t>corrected_correct_comment</t>
+  </si>
+  <si>
+    <t>correction_correct_comment</t>
+  </si>
+  <si>
+    <t>Any comments about above label</t>
+  </si>
+  <si>
+    <t>Tricky, because the whole second part of the sentence (', suggesting…') is problematic</t>
+  </si>
+  <si>
+    <t>whereas' from the originial statement might still be problematic because it suggests that the significant and nonsignificant result are conflicting…</t>
+  </si>
+  <si>
+    <t>LLM just added stuff that actually makes the statement less correct; not 'super incorrect' though</t>
+  </si>
+  <si>
+    <t>Very nice example for a very good correction!</t>
+  </si>
+  <si>
+    <t>LLM adds random stuff, but statement is still correct</t>
+  </si>
+  <si>
+    <t>LLM added too much; the 'do not provide evidence' bit is a little too far</t>
+  </si>
+  <si>
+    <t>again, still incorrectly assumes that sig and nonsig findings are conflicting</t>
+  </si>
+  <si>
+    <t>'no significant evidence' sounds a little strange, but I guess it's okay</t>
+  </si>
+  <si>
+    <t>'sig and nonsig findings are conflicting'</t>
+  </si>
+  <si>
+    <t>really borderline; '…revealed that there was no sig effect' should be 'did not reveal…'; I would have coded 'revealed no sig effect' as 0, so this one as well</t>
+  </si>
+  <si>
+    <t>not perfect, but still nice addition</t>
+  </si>
+  <si>
+    <t>'conflicting sig and nonsig effect'</t>
+  </si>
+  <si>
+    <t>rather complex one; LLM would need to see the conection of the first part to the nonsig. Finding</t>
+  </si>
+  <si>
+    <t>This one's funny; maybe include in article?</t>
+  </si>
+  <si>
+    <t>might actually be an interpretation of an effect size</t>
+  </si>
+  <si>
+    <t>LLM just accepts something like 'was statistically comparable'</t>
+  </si>
+  <si>
+    <t>Maybe the LLM doesn't get that the different parts are connected?</t>
+  </si>
+  <si>
+    <t>really borderline for me; the 'similar' here really feels like an interpretation of the raw means; might also be coded as 0 by someone else</t>
+  </si>
+  <si>
+    <t>last bit still incorrect</t>
+  </si>
+  <si>
+    <t>Another example of LLM being like 'what else do you want me to say???'</t>
+  </si>
+  <si>
+    <t>Should be at least 'did not change significantly' and then no 'indicating…'</t>
+  </si>
+  <si>
+    <t>LLM doesn't like to change 'similarly' etc.</t>
+  </si>
+  <si>
+    <t>still accapting that groups were comparable, but that's a different problem, I guess…</t>
+  </si>
+  <si>
+    <t>nice one Chat!</t>
+  </si>
+  <si>
+    <t>Made it worse… again…</t>
+  </si>
+  <si>
+    <t>I'll give it a 0, but 'did not significantly imagine' is for sure a very strange way of saying it's not significant</t>
+  </si>
+  <si>
+    <t>nice correction!</t>
+  </si>
+  <si>
+    <t>it did correct the 'no effect' bit, but left the conclusion at the end</t>
   </si>
 </sst>
 </file>
@@ -952,7 +1087,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1067,6 +1202,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1112,8 +1305,35 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1489,1121 +1709,1659 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC24B177-1069-49AB-B20A-DC9D80522DC8}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="57.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="8">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="8">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" s="8">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="8">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D25" s="8">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="8">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="8">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="8">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="D28" s="8">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" s="8">
+        <v>0</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" s="8">
+        <v>0</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="D30" s="8">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B31" s="8">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="D31" s="8">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B32" s="8">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B33" s="8">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D33" s="8">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B34" s="8">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="D34" s="8">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B35" s="8">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D35" s="8">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B36" s="8">
+        <v>0</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="D36" s="8">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B37" s="8">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="D37" s="8">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" s="8">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="D38" s="8">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B39" s="8">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="D39" s="8">
+        <v>1</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B40" s="8">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="D40" s="8">
+        <v>0</v>
+      </c>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B41" s="8">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="D41" s="8">
+        <v>1</v>
+      </c>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B42" s="8">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="D42" s="8">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B43" s="8">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="D43" s="8">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B44" s="8">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="D44" s="8">
+        <v>0</v>
+      </c>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B45" s="8">
+        <v>1</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="D45" s="8">
+        <v>1</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B46" s="8">
+        <v>1</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="D46" s="8">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B47" s="8">
+        <v>1</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="D47" s="8">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B48" s="8">
+        <v>1</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="D48" s="8">
+        <v>0</v>
+      </c>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B49" s="8">
+        <v>0</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="D49" s="8">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="B50" s="8">
+        <v>0</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="D50" s="8">
+        <v>0</v>
+      </c>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B51" s="8">
+        <v>1</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="D51" s="8">
+        <v>0</v>
+      </c>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B52" s="8">
+        <v>0</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="D52" s="8">
+        <v>0</v>
+      </c>
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="B53" s="8">
+        <v>1</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="D53" s="8">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="B54" s="8">
+        <v>1</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="D54" s="8">
+        <v>1</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B55" s="8">
+        <v>1</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="D55" s="8">
+        <v>0</v>
+      </c>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B56" s="8">
+        <v>1</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="D56" s="8">
+        <v>0</v>
+      </c>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B57" s="8">
+        <v>1</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="D57" s="8">
+        <v>1</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B58" s="8">
+        <v>1</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="D58" s="8">
+        <v>0</v>
+      </c>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B59" s="8">
+        <v>1</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="D59" s="8">
+        <v>1</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B60" s="8">
+        <v>1</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="D60" s="8">
+        <v>0</v>
+      </c>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B61" s="8">
+        <v>1</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="D61" s="8">
+        <v>1</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B62" s="8">
+        <v>0</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="D62" s="8">
+        <v>0</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B63" s="8">
+        <v>1</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="D63" s="8">
+        <v>0</v>
+      </c>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B64" s="8">
+        <v>1</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="D64" s="8">
+        <v>1</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B65" s="8">
+        <v>1</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="D65" s="8">
+        <v>0</v>
+      </c>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="B66" s="8">
+        <v>1</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="D66" s="8">
+        <v>0</v>
+      </c>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B67" s="8">
+        <v>1</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="D67" s="8">
+        <v>0</v>
+      </c>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B68" s="8">
+        <v>1</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="D68" s="8">
+        <v>0</v>
+      </c>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B69" s="8">
+        <v>1</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="D69" s="8">
+        <v>1</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="B70" s="8">
+        <v>0</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="D70" s="8">
+        <v>0</v>
+      </c>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B71" s="8">
+        <v>1</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="D71" s="8">
+        <v>0</v>
+      </c>
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B72" s="8">
+        <v>1</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="D72" s="8">
+        <v>0</v>
+      </c>
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B73" s="8">
+        <v>1</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="D73" s="8">
+        <v>0</v>
+      </c>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B74">
-        <v>1</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="B74" s="8">
+        <v>1</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="D74" s="8">
+        <v>0</v>
+      </c>
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="B75" s="8">
+        <v>1</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="D75" s="8">
+        <v>0</v>
+      </c>
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B76">
-        <v>0</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="B76" s="8">
+        <v>0</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="D76" s="8">
+        <v>0</v>
+      </c>
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="B77" s="8">
+        <v>1</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="D77" s="8">
+        <v>0</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="B78" s="8">
+        <v>1</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="D78" s="8">
+        <v>0</v>
+      </c>
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B79">
-        <v>1</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="B79" s="8">
+        <v>1</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="D79" s="8">
+        <v>0</v>
+      </c>
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B80">
-        <v>0</v>
-      </c>
-      <c r="C80" t="s">
+      <c r="B80" s="8">
+        <v>0</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="D80" s="8">
+        <v>0</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B81">
-        <v>0</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="B81" s="8">
+        <v>0</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="D81" s="8">
+        <v>1</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B82">
-        <v>1</v>
-      </c>
-      <c r="C82" t="s">
+      <c r="B82" s="8">
+        <v>1</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="D82" s="8">
+        <v>0</v>
+      </c>
+      <c r="E82" s="4"/>
+    </row>
+    <row r="83" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B83">
-        <v>0</v>
-      </c>
-      <c r="C83" t="s">
+      <c r="B83" s="8">
+        <v>0</v>
+      </c>
+      <c r="C83" s="4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="D83" s="8">
+        <v>0</v>
+      </c>
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B84">
-        <v>1</v>
-      </c>
-      <c r="C84" t="s">
+      <c r="B84" s="8">
+        <v>1</v>
+      </c>
+      <c r="C84" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="D84" s="8">
+        <v>0</v>
+      </c>
+      <c r="E84" s="4"/>
+    </row>
+    <row r="85" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B85">
-        <v>0</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="B85" s="8">
+        <v>0</v>
+      </c>
+      <c r="C85" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="D85" s="8">
+        <v>0</v>
+      </c>
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B86">
-        <v>1</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="B86" s="8">
+        <v>1</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="D86" s="8">
+        <v>0</v>
+      </c>
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B87">
-        <v>1</v>
-      </c>
-      <c r="C87" t="s">
+      <c r="B87" s="8">
+        <v>1</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="D87" s="8">
+        <v>0</v>
+      </c>
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B88">
-        <v>1</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="B88" s="8">
+        <v>1</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="D88" s="8">
+        <v>0</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B89">
-        <v>1</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="B89" s="8">
+        <v>1</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="D89" s="8">
+        <v>0</v>
+      </c>
+      <c r="E89" s="4"/>
+    </row>
+    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B90">
-        <v>1</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="B90" s="8">
+        <v>1</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="D90" s="8">
+        <v>0</v>
+      </c>
+      <c r="E90" s="4"/>
+    </row>
+    <row r="91" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B91">
-        <v>1</v>
-      </c>
-      <c r="C91" t="s">
+      <c r="B91" s="8">
+        <v>1</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="D91" s="8">
+        <v>0</v>
+      </c>
+      <c r="E91" s="4"/>
+    </row>
+    <row r="92" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B92">
-        <v>1</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="B92" s="8">
+        <v>1</v>
+      </c>
+      <c r="C92" s="4" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="D92" s="8">
+        <v>0</v>
+      </c>
+      <c r="E92" s="4"/>
+    </row>
+    <row r="93" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B93">
-        <v>1</v>
-      </c>
-      <c r="C93" t="s">
+      <c r="B93" s="8">
+        <v>1</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="D93" s="8">
+        <v>0</v>
+      </c>
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B94">
-        <v>1</v>
-      </c>
-      <c r="C94" t="s">
+      <c r="B94" s="8">
+        <v>1</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="D94" s="8">
+        <v>0</v>
+      </c>
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B95">
-        <v>1</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="B95" s="8">
+        <v>1</v>
+      </c>
+      <c r="C95" s="4" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="D95" s="8">
+        <v>0</v>
+      </c>
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B96">
-        <v>1</v>
-      </c>
-      <c r="C96" t="s">
+      <c r="B96" s="8">
+        <v>1</v>
+      </c>
+      <c r="C96" s="4" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="D96" s="8">
+        <v>0</v>
+      </c>
+      <c r="E96" s="4"/>
+    </row>
+    <row r="97" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-      <c r="C97" t="s">
+      <c r="B97" s="8">
+        <v>1</v>
+      </c>
+      <c r="C97" s="4" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="D97" s="8">
+        <v>0</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B98">
-        <v>0</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="B98" s="8">
+        <v>0</v>
+      </c>
+      <c r="C98" s="4" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="D98" s="8">
+        <v>0</v>
+      </c>
+      <c r="E98" s="4"/>
+    </row>
+    <row r="99" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B99">
-        <v>1</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="B99" s="8">
+        <v>1</v>
+      </c>
+      <c r="C99" s="4" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="D99" s="8">
+        <v>0</v>
+      </c>
+      <c r="E99" s="4"/>
+    </row>
+    <row r="100" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B100">
-        <v>1</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="B100" s="8">
+        <v>1</v>
+      </c>
+      <c r="C100" s="4" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="D100" s="8">
+        <v>0</v>
+      </c>
+      <c r="E100" s="4"/>
+    </row>
+    <row r="101" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B101">
-        <v>1</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="B101" s="8">
+        <v>1</v>
+      </c>
+      <c r="C101" s="4" t="s">
         <v>202</v>
+      </c>
+      <c r="D101" s="8">
+        <v>1</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6630B625-93BC-4617-8016-437EA6DFD602}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>